<commit_message>
Count error occurrences and formatted into dataframe
</commit_message>
<xml_diff>
--- a/file1.xlsx
+++ b/file1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uzair\Desktop\Work\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68D4A754-E577-4F1D-A44F-F34C4AA558FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838CB5DE-3784-4025-947E-0F49C091455E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{58F0D9BD-14BE-43F6-9692-9E55450D4BC6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Heading 1</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Heading 4</t>
+  </si>
+  <si>
+    <t>lrs-200 JOB Failure</t>
+  </si>
+  <si>
+    <t>mcc.prod_INC 3398  ALARM</t>
+  </si>
+  <si>
+    <t>MAX_RUNTIME</t>
   </si>
 </sst>
 </file>
@@ -422,10 +431,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="19.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -451,7 +463,7 @@
       <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -465,8 +477,8 @@
       <c r="C3" s="2">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
-        <v>8</v>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -479,8 +491,8 @@
       <c r="C4" s="2">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
-        <v>12</v>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added graphing and better demo files
</commit_message>
<xml_diff>
--- a/file1.xlsx
+++ b/file1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uzair\Desktop\Work\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838CB5DE-3784-4025-947E-0F49C091455E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9265F84-C39A-4ABC-B549-02F70B4709E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{58F0D9BD-14BE-43F6-9692-9E55450D4BC6}"/>
   </bookViews>
@@ -31,34 +31,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Heading 1</t>
-  </si>
-  <si>
-    <t>Heading 2</t>
-  </si>
-  <si>
-    <t>Heading 3</t>
-  </si>
-  <si>
-    <t>Heading 4</t>
-  </si>
-  <si>
-    <t>lrs-200 JOB Failure</t>
-  </si>
-  <si>
-    <t>mcc.prod_INC 3398  ALARM</t>
-  </si>
-  <si>
-    <t>MAX_RUNTIME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>JobName</t>
+  </si>
+  <si>
+    <t>MessageAlert</t>
+  </si>
+  <si>
+    <t>STARS</t>
+  </si>
+  <si>
+    <t>app-random_error</t>
+  </si>
+  <si>
+    <t>AUTOSYS ALARM: WATCHFAILURE, JOB: app-random_error</t>
+  </si>
+  <si>
+    <t>DVP</t>
+  </si>
+  <si>
+    <t>app-lrs-200-setup_launch</t>
+  </si>
+  <si>
+    <t>AUTOSYS ALARM: JOB_FAILURE, JOB: app-lrs-200-setup_launch</t>
+  </si>
+  <si>
+    <t>OMR</t>
+  </si>
+  <si>
+    <t>app-system-upload</t>
+  </si>
+  <si>
+    <t>AUTOSYS ALARM: MAX_RUNTIME, JOB: app-system-upload</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>INC0027</t>
+  </si>
+  <si>
+    <t>INC0028</t>
+  </si>
+  <si>
+    <t>INC0029</t>
+  </si>
+  <si>
+    <t>INC0030</t>
+  </si>
+  <si>
+    <t>INC0031</t>
+  </si>
+  <si>
+    <t>INC0032</t>
+  </si>
+  <si>
+    <t>INC0033</t>
+  </si>
+  <si>
+    <t>INC0034</t>
+  </si>
+  <si>
+    <t>INC0035</t>
+  </si>
+  <si>
+    <t>INC0036</t>
+  </si>
+  <si>
+    <t>INC0037</t>
+  </si>
+  <si>
+    <t>INC0038</t>
+  </si>
+  <si>
+    <t>INC0039</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +140,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -83,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,14 +178,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,18 +513,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F476CB06-81BC-4429-AE97-5102B6612F13}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="19.9296875" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,50 +540,275 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43591</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43592</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43593</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="D5" s="3">
+        <v>43594</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43595</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D7" s="3">
+        <v>43596</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <v>43597</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
+      <c r="D9" s="3">
+        <v>43598</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43599</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43600</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43601</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43602</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43603</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>